<commit_message>
Updated documentation for final delivery
Sequence diagrams updated for refactoring
Class diagram updated for refactoring also
System test cases redone to include input and output using images of the ui
Other Development docs updated and cleaned up for final delivery
Package Diagram redone to include ineractions between packages
Domain Model did not require any changes

Note: Doxygen will be updated in a separate commit
</commit_message>
<xml_diff>
--- a/Documentation/Development Docs/Traceability Link Matrix.xlsx
+++ b/Documentation/Development Docs/Traceability Link Matrix.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="106">
   <si>
     <t>UC-00</t>
   </si>
@@ -309,6 +309,30 @@
   </si>
   <si>
     <t>ModifyRoutine</t>
+  </si>
+  <si>
+    <t>UC-13</t>
+  </si>
+  <si>
+    <t>UC-14</t>
+  </si>
+  <si>
+    <t>UC-15</t>
+  </si>
+  <si>
+    <t>UC-16</t>
+  </si>
+  <si>
+    <t>UC-17</t>
+  </si>
+  <si>
+    <t>UC-18</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>Remove</t>
   </si>
 </sst>
 </file>
@@ -708,10 +732,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:BB25"/>
+  <dimension ref="B2:BB31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1501,9 +1525,7 @@
       <c r="AB7" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="AC7" s="4" t="s">
-        <v>54</v>
-      </c>
+      <c r="AC7" s="4"/>
       <c r="AD7" s="4"/>
       <c r="AE7" s="4" t="s">
         <v>54</v>
@@ -1582,9 +1604,7 @@
       <c r="AB8" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="AC8" s="4" t="s">
-        <v>54</v>
-      </c>
+      <c r="AC8" s="4"/>
       <c r="AD8" s="4"/>
       <c r="AE8" s="4" t="s">
         <v>54</v>
@@ -1665,9 +1685,7 @@
       <c r="AB9" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="AC9" s="4" t="s">
-        <v>54</v>
-      </c>
+      <c r="AC9" s="4"/>
       <c r="AD9" s="4"/>
       <c r="AE9" s="4" t="s">
         <v>54</v>
@@ -1920,9 +1938,7 @@
         <v>54</v>
       </c>
       <c r="AB12" s="4"/>
-      <c r="AC12" s="4" t="s">
-        <v>54</v>
-      </c>
+      <c r="AC12" s="4"/>
       <c r="AD12" s="4"/>
       <c r="AE12" s="4" t="s">
         <v>54</v>
@@ -2163,9 +2179,7 @@
       <c r="Z15" s="4"/>
       <c r="AA15" s="4"/>
       <c r="AB15" s="4"/>
-      <c r="AC15" s="4" t="s">
-        <v>54</v>
-      </c>
+      <c r="AC15" s="4"/>
       <c r="AD15" s="4"/>
       <c r="AE15" s="4" t="s">
         <v>54</v>
@@ -2388,9 +2402,7 @@
       <c r="Z18" s="4"/>
       <c r="AA18" s="4"/>
       <c r="AB18" s="4"/>
-      <c r="AC18" s="4" t="s">
-        <v>54</v>
-      </c>
+      <c r="AC18" s="4"/>
       <c r="AD18" s="4"/>
       <c r="AE18" s="4" t="s">
         <v>54</v>
@@ -2651,9 +2663,7 @@
       <c r="Z21" s="4"/>
       <c r="AA21" s="4"/>
       <c r="AB21" s="4"/>
-      <c r="AC21" s="4" t="s">
-        <v>54</v>
-      </c>
+      <c r="AC21" s="4"/>
       <c r="AD21" s="4"/>
       <c r="AE21" s="4" t="s">
         <v>54</v>
@@ -2916,9 +2926,7 @@
       <c r="Z24" s="4"/>
       <c r="AA24" s="4"/>
       <c r="AB24" s="4"/>
-      <c r="AC24" s="4" t="s">
-        <v>54</v>
-      </c>
+      <c r="AC24" s="4"/>
       <c r="AD24" s="4"/>
       <c r="AE24" s="4" t="s">
         <v>54</v>
@@ -3036,6 +3044,446 @@
         <v>54</v>
       </c>
     </row>
+    <row r="26" spans="2:54">
+      <c r="B26" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="4"/>
+      <c r="S26" s="4"/>
+      <c r="T26" s="4"/>
+      <c r="U26" s="4"/>
+      <c r="V26" s="4"/>
+      <c r="W26" s="4"/>
+      <c r="X26" s="4"/>
+      <c r="Y26" s="4"/>
+      <c r="Z26" s="4"/>
+      <c r="AA26" s="4"/>
+      <c r="AB26" s="4"/>
+      <c r="AC26" s="4"/>
+      <c r="AD26" s="4"/>
+      <c r="AE26" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF26" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG26" s="4"/>
+      <c r="AH26" s="4"/>
+      <c r="AI26" s="4"/>
+      <c r="AJ26" s="4"/>
+      <c r="AK26" s="4"/>
+      <c r="AL26" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM26" s="4"/>
+      <c r="AN26" s="4"/>
+      <c r="AO26" s="4"/>
+      <c r="AP26" s="4"/>
+      <c r="AQ26" s="4"/>
+      <c r="AR26" s="4"/>
+      <c r="AS26" s="4"/>
+      <c r="AT26" s="4"/>
+      <c r="AU26" s="4"/>
+      <c r="AV26" s="4"/>
+      <c r="AW26" s="4"/>
+      <c r="AX26" s="4"/>
+      <c r="AY26" s="4"/>
+      <c r="AZ26" s="4"/>
+      <c r="BA26" s="4"/>
+      <c r="BB26" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="2:54">
+      <c r="B27" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="4"/>
+      <c r="S27" s="4"/>
+      <c r="T27" s="4"/>
+      <c r="U27" s="4"/>
+      <c r="V27" s="4"/>
+      <c r="W27" s="4"/>
+      <c r="X27" s="4"/>
+      <c r="Y27" s="4"/>
+      <c r="Z27" s="4"/>
+      <c r="AA27" s="4"/>
+      <c r="AB27" s="4"/>
+      <c r="AC27" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD27" s="4"/>
+      <c r="AE27" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF27" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG27" s="4"/>
+      <c r="AH27" s="4"/>
+      <c r="AI27" s="4"/>
+      <c r="AJ27" s="4"/>
+      <c r="AK27" s="4"/>
+      <c r="AL27" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM27" s="4"/>
+      <c r="AN27" s="4"/>
+      <c r="AO27" s="4"/>
+      <c r="AP27" s="4"/>
+      <c r="AQ27" s="4"/>
+      <c r="AR27" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS27" s="4"/>
+      <c r="AT27" s="4"/>
+      <c r="AU27" s="4"/>
+      <c r="AV27" s="4"/>
+      <c r="AW27" s="4"/>
+      <c r="AX27" s="4"/>
+      <c r="AY27" s="4"/>
+      <c r="AZ27" s="4"/>
+      <c r="BA27" s="4"/>
+      <c r="BB27" s="4"/>
+    </row>
+    <row r="28" spans="2:54">
+      <c r="B28" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="4"/>
+      <c r="T28" s="4"/>
+      <c r="U28" s="4"/>
+      <c r="V28" s="4"/>
+      <c r="W28" s="4"/>
+      <c r="X28" s="4"/>
+      <c r="Y28" s="4"/>
+      <c r="Z28" s="4"/>
+      <c r="AA28" s="4"/>
+      <c r="AB28" s="4"/>
+      <c r="AC28" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD28" s="4"/>
+      <c r="AE28" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF28" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG28" s="4"/>
+      <c r="AH28" s="4"/>
+      <c r="AI28" s="4"/>
+      <c r="AJ28" s="4"/>
+      <c r="AK28" s="4"/>
+      <c r="AL28" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM28" s="4"/>
+      <c r="AN28" s="4"/>
+      <c r="AO28" s="4"/>
+      <c r="AP28" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ28" s="4"/>
+      <c r="AR28" s="4"/>
+      <c r="AS28" s="4"/>
+      <c r="AT28" s="4"/>
+      <c r="AU28" s="4"/>
+      <c r="AV28" s="4"/>
+      <c r="AW28" s="4"/>
+      <c r="AX28" s="4"/>
+      <c r="AY28" s="4"/>
+      <c r="AZ28" s="4"/>
+      <c r="BA28" s="4"/>
+      <c r="BB28" s="4"/>
+    </row>
+    <row r="29" spans="2:54">
+      <c r="B29" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="4"/>
+      <c r="U29" s="4"/>
+      <c r="V29" s="4"/>
+      <c r="W29" s="4"/>
+      <c r="X29" s="4"/>
+      <c r="Y29" s="4"/>
+      <c r="Z29" s="4"/>
+      <c r="AA29" s="4"/>
+      <c r="AB29" s="4"/>
+      <c r="AC29" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD29" s="4"/>
+      <c r="AE29" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF29" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG29" s="4"/>
+      <c r="AH29" s="4"/>
+      <c r="AI29" s="4"/>
+      <c r="AJ29" s="4"/>
+      <c r="AK29" s="4"/>
+      <c r="AL29" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM29" s="4"/>
+      <c r="AN29" s="4"/>
+      <c r="AO29" s="4"/>
+      <c r="AP29" s="4"/>
+      <c r="AQ29" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR29" s="4"/>
+      <c r="AS29" s="4"/>
+      <c r="AT29" s="4"/>
+      <c r="AU29" s="4"/>
+      <c r="AV29" s="4"/>
+      <c r="AW29" s="4"/>
+      <c r="AX29" s="4"/>
+      <c r="AY29" s="4"/>
+      <c r="AZ29" s="4"/>
+      <c r="BA29" s="4"/>
+      <c r="BB29" s="4"/>
+    </row>
+    <row r="30" spans="2:54">
+      <c r="B30" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="4"/>
+      <c r="Q30" s="4"/>
+      <c r="R30" s="4"/>
+      <c r="S30" s="4"/>
+      <c r="T30" s="4"/>
+      <c r="U30" s="4"/>
+      <c r="V30" s="4"/>
+      <c r="W30" s="4"/>
+      <c r="X30" s="4"/>
+      <c r="Y30" s="4"/>
+      <c r="Z30" s="4"/>
+      <c r="AA30" s="4"/>
+      <c r="AB30" s="4"/>
+      <c r="AC30" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD30" s="4"/>
+      <c r="AE30" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF30" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG30" s="4"/>
+      <c r="AH30" s="4"/>
+      <c r="AI30" s="4"/>
+      <c r="AJ30" s="4"/>
+      <c r="AK30" s="4"/>
+      <c r="AL30" s="4"/>
+      <c r="AM30" s="4"/>
+      <c r="AN30" s="4"/>
+      <c r="AO30" s="4"/>
+      <c r="AP30" s="4"/>
+      <c r="AQ30" s="4"/>
+      <c r="AR30" s="4"/>
+      <c r="AS30" s="4"/>
+      <c r="AT30" s="4"/>
+      <c r="AU30" s="4"/>
+      <c r="AV30" s="4"/>
+      <c r="AW30" s="4"/>
+      <c r="AX30" s="4"/>
+      <c r="AY30" s="4"/>
+      <c r="AZ30" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="BA30" s="4"/>
+      <c r="BB30" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="2:54">
+      <c r="B31" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4"/>
+      <c r="R31" s="4"/>
+      <c r="S31" s="4"/>
+      <c r="T31" s="4"/>
+      <c r="U31" s="4"/>
+      <c r="V31" s="4"/>
+      <c r="W31" s="4"/>
+      <c r="X31" s="4"/>
+      <c r="Y31" s="4"/>
+      <c r="Z31" s="4"/>
+      <c r="AA31" s="4"/>
+      <c r="AB31" s="4"/>
+      <c r="AC31" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD31" s="4"/>
+      <c r="AE31" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF31" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG31" s="4"/>
+      <c r="AH31" s="4"/>
+      <c r="AI31" s="4"/>
+      <c r="AJ31" s="4"/>
+      <c r="AK31" s="4"/>
+      <c r="AL31" s="4"/>
+      <c r="AM31" s="4"/>
+      <c r="AN31" s="4"/>
+      <c r="AO31" s="4"/>
+      <c r="AP31" s="4"/>
+      <c r="AQ31" s="4"/>
+      <c r="AR31" s="4"/>
+      <c r="AS31" s="4"/>
+      <c r="AT31" s="4"/>
+      <c r="AU31" s="4"/>
+      <c r="AV31" s="4"/>
+      <c r="AW31" s="4"/>
+      <c r="AX31" s="4"/>
+      <c r="AY31" s="4"/>
+      <c r="AZ31" s="4"/>
+      <c r="BA31" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="BB31" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3043,10 +3491,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:AA55"/>
+  <dimension ref="B1:AG55"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:Y55"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AE55" sqref="B3:AE55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3064,10 +3512,15 @@
     <col min="16" max="18" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="19" max="21" width="8.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="22" max="25" width="8" style="3" customWidth="1"/>
-    <col min="26" max="16384" width="9.140625" style="3"/>
+    <col min="26" max="26" width="7" style="3" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="8.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:27">
+    <row r="1" spans="2:33">
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -3093,8 +3546,14 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
-    </row>
-    <row r="3" spans="2:27">
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
+      <c r="AG1" s="1"/>
+    </row>
+    <row r="3" spans="2:33">
       <c r="F3" s="2" t="s">
         <v>66</v>
       </c>
@@ -3155,8 +3614,26 @@
       <c r="Y3" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="4" spans="2:27">
+      <c r="Z3" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AD3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="2:33">
       <c r="F4" s="2" t="s">
         <v>72</v>
       </c>
@@ -3217,8 +3694,26 @@
       <c r="Y4" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="2:27">
+      <c r="Z4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AD4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="2:33">
       <c r="B5" s="6" t="s">
         <v>63</v>
       </c>
@@ -3291,8 +3786,26 @@
       <c r="Y5" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="2:27">
+      <c r="Z5" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="AA5" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB5" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC5" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD5" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="AE5" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="2:33">
       <c r="B6" s="4" t="s">
         <v>59</v>
       </c>
@@ -3331,8 +3844,18 @@
       <c r="Y6" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="7" spans="2:27">
+      <c r="Z6" s="4"/>
+      <c r="AA6" s="4"/>
+      <c r="AB6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC6" s="4"/>
+      <c r="AD6" s="4"/>
+      <c r="AE6" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="2:33">
       <c r="B7" s="4" t="s">
         <v>59</v>
       </c>
@@ -3373,8 +3896,16 @@
       <c r="W7" s="4"/>
       <c r="X7" s="4"/>
       <c r="Y7" s="4"/>
-    </row>
-    <row r="8" spans="2:27">
+      <c r="Z7" s="4"/>
+      <c r="AA7" s="4"/>
+      <c r="AB7" s="4"/>
+      <c r="AC7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD7" s="4"/>
+      <c r="AE7" s="4"/>
+    </row>
+    <row r="8" spans="2:33">
       <c r="B8" s="4" t="s">
         <v>59</v>
       </c>
@@ -3415,8 +3946,18 @@
       </c>
       <c r="X8" s="4"/>
       <c r="Y8" s="4"/>
-    </row>
-    <row r="9" spans="2:27">
+      <c r="Z8" s="4"/>
+      <c r="AA8" s="4"/>
+      <c r="AB8" s="4"/>
+      <c r="AC8" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD8" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE8" s="4"/>
+    </row>
+    <row r="9" spans="2:33">
       <c r="B9" s="4" t="s">
         <v>59</v>
       </c>
@@ -3455,8 +3996,14 @@
       <c r="W9" s="4"/>
       <c r="X9" s="4"/>
       <c r="Y9" s="4"/>
-    </row>
-    <row r="10" spans="2:27">
+      <c r="Z9" s="4"/>
+      <c r="AA9" s="4"/>
+      <c r="AB9" s="4"/>
+      <c r="AC9" s="4"/>
+      <c r="AD9" s="4"/>
+      <c r="AE9" s="4"/>
+    </row>
+    <row r="10" spans="2:33">
       <c r="B10" s="4" t="s">
         <v>59</v>
       </c>
@@ -3495,8 +4042,18 @@
       <c r="Y10" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="11" spans="2:27">
+      <c r="Z10" s="4"/>
+      <c r="AA10" s="4"/>
+      <c r="AB10" s="4"/>
+      <c r="AC10" s="4"/>
+      <c r="AD10" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE10" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="2:33">
       <c r="B11" s="4" t="s">
         <v>59</v>
       </c>
@@ -3551,8 +4108,16 @@
         <v>54</v>
       </c>
       <c r="Y11" s="4"/>
-    </row>
-    <row r="12" spans="2:27">
+      <c r="Z11" s="4"/>
+      <c r="AA11" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB11" s="4"/>
+      <c r="AC11" s="4"/>
+      <c r="AD11" s="4"/>
+      <c r="AE11" s="4"/>
+    </row>
+    <row r="12" spans="2:33">
       <c r="B12" s="4" t="s">
         <v>59</v>
       </c>
@@ -3603,8 +4168,14 @@
         <v>54</v>
       </c>
       <c r="Y12" s="4"/>
-    </row>
-    <row r="13" spans="2:27">
+      <c r="Z12" s="4"/>
+      <c r="AA12" s="4"/>
+      <c r="AB12" s="4"/>
+      <c r="AC12" s="4"/>
+      <c r="AD12" s="4"/>
+      <c r="AE12" s="4"/>
+    </row>
+    <row r="13" spans="2:33">
       <c r="B13" s="4" t="s">
         <v>59</v>
       </c>
@@ -3649,8 +4220,14 @@
         <v>54</v>
       </c>
       <c r="Y13" s="4"/>
-    </row>
-    <row r="14" spans="2:27">
+      <c r="Z13" s="4"/>
+      <c r="AA13" s="4"/>
+      <c r="AB13" s="4"/>
+      <c r="AC13" s="4"/>
+      <c r="AD13" s="4"/>
+      <c r="AE13" s="4"/>
+    </row>
+    <row r="14" spans="2:33">
       <c r="B14" s="4" t="s">
         <v>59</v>
       </c>
@@ -3695,8 +4272,14 @@
         <v>54</v>
       </c>
       <c r="Y14" s="4"/>
-    </row>
-    <row r="15" spans="2:27">
+      <c r="Z14" s="4"/>
+      <c r="AA14" s="4"/>
+      <c r="AB14" s="4"/>
+      <c r="AC14" s="4"/>
+      <c r="AD14" s="4"/>
+      <c r="AE14" s="4"/>
+    </row>
+    <row r="15" spans="2:33">
       <c r="B15" s="4" t="s">
         <v>59</v>
       </c>
@@ -3735,8 +4318,14 @@
         <v>54</v>
       </c>
       <c r="Y15" s="4"/>
-    </row>
-    <row r="16" spans="2:27">
+      <c r="Z15" s="4"/>
+      <c r="AA15" s="4"/>
+      <c r="AB15" s="4"/>
+      <c r="AC15" s="4"/>
+      <c r="AD15" s="4"/>
+      <c r="AE15" s="4"/>
+    </row>
+    <row r="16" spans="2:33">
       <c r="B16" s="4" t="s">
         <v>59</v>
       </c>
@@ -3781,8 +4370,14 @@
         <v>54</v>
       </c>
       <c r="Y16" s="4"/>
-    </row>
-    <row r="17" spans="2:25">
+      <c r="Z16" s="4"/>
+      <c r="AA16" s="4"/>
+      <c r="AB16" s="4"/>
+      <c r="AC16" s="4"/>
+      <c r="AD16" s="4"/>
+      <c r="AE16" s="4"/>
+    </row>
+    <row r="17" spans="2:31">
       <c r="B17" s="4" t="s">
         <v>59</v>
       </c>
@@ -3827,8 +4422,14 @@
         <v>54</v>
       </c>
       <c r="Y17" s="4"/>
-    </row>
-    <row r="18" spans="2:25">
+      <c r="Z17" s="4"/>
+      <c r="AA17" s="4"/>
+      <c r="AB17" s="4"/>
+      <c r="AC17" s="4"/>
+      <c r="AD17" s="4"/>
+      <c r="AE17" s="4"/>
+    </row>
+    <row r="18" spans="2:31">
       <c r="B18" s="4" t="s">
         <v>59</v>
       </c>
@@ -3871,8 +4472,14 @@
       <c r="W18" s="4"/>
       <c r="X18" s="4"/>
       <c r="Y18" s="4"/>
-    </row>
-    <row r="19" spans="2:25">
+      <c r="Z18" s="4"/>
+      <c r="AA18" s="4"/>
+      <c r="AB18" s="4"/>
+      <c r="AC18" s="4"/>
+      <c r="AD18" s="4"/>
+      <c r="AE18" s="4"/>
+    </row>
+    <row r="19" spans="2:31">
       <c r="B19" s="4" t="s">
         <v>59</v>
       </c>
@@ -3915,8 +4522,14 @@
       <c r="W19" s="4"/>
       <c r="X19" s="4"/>
       <c r="Y19" s="4"/>
-    </row>
-    <row r="20" spans="2:25">
+      <c r="Z19" s="4"/>
+      <c r="AA19" s="4"/>
+      <c r="AB19" s="4"/>
+      <c r="AC19" s="4"/>
+      <c r="AD19" s="4"/>
+      <c r="AE19" s="4"/>
+    </row>
+    <row r="20" spans="2:31">
       <c r="B20" s="4" t="s">
         <v>59</v>
       </c>
@@ -3953,8 +4566,14 @@
       <c r="W20" s="4"/>
       <c r="X20" s="4"/>
       <c r="Y20" s="4"/>
-    </row>
-    <row r="21" spans="2:25">
+      <c r="Z20" s="4"/>
+      <c r="AA20" s="4"/>
+      <c r="AB20" s="4"/>
+      <c r="AC20" s="4"/>
+      <c r="AD20" s="4"/>
+      <c r="AE20" s="4"/>
+    </row>
+    <row r="21" spans="2:31">
       <c r="B21" s="4" t="s">
         <v>59</v>
       </c>
@@ -4007,8 +4626,14 @@
       <c r="Y21" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="22" spans="2:25">
+      <c r="Z21" s="4"/>
+      <c r="AA21" s="4"/>
+      <c r="AB21" s="4"/>
+      <c r="AC21" s="4"/>
+      <c r="AD21" s="4"/>
+      <c r="AE21" s="4"/>
+    </row>
+    <row r="22" spans="2:31">
       <c r="B22" s="4" t="s">
         <v>59</v>
       </c>
@@ -4045,8 +4670,14 @@
       <c r="W22" s="4"/>
       <c r="X22" s="4"/>
       <c r="Y22" s="4"/>
-    </row>
-    <row r="23" spans="2:25">
+      <c r="Z22" s="4"/>
+      <c r="AA22" s="4"/>
+      <c r="AB22" s="4"/>
+      <c r="AC22" s="4"/>
+      <c r="AD22" s="4"/>
+      <c r="AE22" s="4"/>
+    </row>
+    <row r="23" spans="2:31">
       <c r="B23" s="4" t="s">
         <v>59</v>
       </c>
@@ -4083,8 +4714,14 @@
       <c r="W23" s="4"/>
       <c r="X23" s="4"/>
       <c r="Y23" s="4"/>
-    </row>
-    <row r="24" spans="2:25">
+      <c r="Z23" s="4"/>
+      <c r="AA23" s="4"/>
+      <c r="AB23" s="4"/>
+      <c r="AC23" s="4"/>
+      <c r="AD23" s="4"/>
+      <c r="AE23" s="4"/>
+    </row>
+    <row r="24" spans="2:31">
       <c r="B24" s="4" t="s">
         <v>59</v>
       </c>
@@ -4121,8 +4758,14 @@
       <c r="W24" s="4"/>
       <c r="X24" s="4"/>
       <c r="Y24" s="4"/>
-    </row>
-    <row r="25" spans="2:25">
+      <c r="Z24" s="4"/>
+      <c r="AA24" s="4"/>
+      <c r="AB24" s="4"/>
+      <c r="AC24" s="4"/>
+      <c r="AD24" s="4"/>
+      <c r="AE24" s="4"/>
+    </row>
+    <row r="25" spans="2:31">
       <c r="B25" s="4" t="s">
         <v>59</v>
       </c>
@@ -4163,8 +4806,14 @@
       <c r="Y25" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="26" spans="2:25">
+      <c r="Z25" s="4"/>
+      <c r="AA25" s="4"/>
+      <c r="AB25" s="4"/>
+      <c r="AC25" s="4"/>
+      <c r="AD25" s="4"/>
+      <c r="AE25" s="4"/>
+    </row>
+    <row r="26" spans="2:31">
       <c r="B26" s="4" t="s">
         <v>59</v>
       </c>
@@ -4205,8 +4854,14 @@
       <c r="W26" s="4"/>
       <c r="X26" s="4"/>
       <c r="Y26" s="4"/>
-    </row>
-    <row r="27" spans="2:25">
+      <c r="Z26" s="4"/>
+      <c r="AA26" s="4"/>
+      <c r="AB26" s="4"/>
+      <c r="AC26" s="4"/>
+      <c r="AD26" s="4"/>
+      <c r="AE26" s="4"/>
+    </row>
+    <row r="27" spans="2:31">
       <c r="B27" s="4" t="s">
         <v>59</v>
       </c>
@@ -4251,8 +4906,14 @@
       <c r="W27" s="4"/>
       <c r="X27" s="4"/>
       <c r="Y27" s="4"/>
-    </row>
-    <row r="28" spans="2:25">
+      <c r="Z27" s="4"/>
+      <c r="AA27" s="4"/>
+      <c r="AB27" s="4"/>
+      <c r="AC27" s="4"/>
+      <c r="AD27" s="4"/>
+      <c r="AE27" s="4"/>
+    </row>
+    <row r="28" spans="2:31">
       <c r="B28" s="4" t="s">
         <v>59</v>
       </c>
@@ -4299,8 +4960,14 @@
       <c r="W28" s="4"/>
       <c r="X28" s="4"/>
       <c r="Y28" s="4"/>
-    </row>
-    <row r="29" spans="2:25">
+      <c r="Z28" s="4"/>
+      <c r="AA28" s="4"/>
+      <c r="AB28" s="4"/>
+      <c r="AC28" s="4"/>
+      <c r="AD28" s="4"/>
+      <c r="AE28" s="4"/>
+    </row>
+    <row r="29" spans="2:31">
       <c r="B29" s="4" t="s">
         <v>59</v>
       </c>
@@ -4337,8 +5004,14 @@
       <c r="W29" s="4"/>
       <c r="X29" s="4"/>
       <c r="Y29" s="4"/>
-    </row>
-    <row r="30" spans="2:25">
+      <c r="Z29" s="4"/>
+      <c r="AA29" s="4"/>
+      <c r="AB29" s="4"/>
+      <c r="AC29" s="4"/>
+      <c r="AD29" s="4"/>
+      <c r="AE29" s="4"/>
+    </row>
+    <row r="30" spans="2:31">
       <c r="B30" s="4" t="s">
         <v>85</v>
       </c>
@@ -4352,65 +5025,65 @@
       <c r="F30" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="G30" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="I30" s="4" t="s">
-        <v>54</v>
-      </c>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
       <c r="J30" s="4" t="s">
         <v>54</v>
       </c>
       <c r="K30" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="L30" s="4" t="s">
-        <v>54</v>
-      </c>
+      <c r="L30" s="4"/>
       <c r="M30" s="4" t="s">
         <v>54</v>
       </c>
       <c r="N30" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="O30" s="4" t="s">
-        <v>54</v>
-      </c>
+      <c r="O30" s="4"/>
       <c r="P30" s="4" t="s">
         <v>54</v>
       </c>
       <c r="Q30" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="R30" s="4" t="s">
-        <v>54</v>
-      </c>
+      <c r="R30" s="4"/>
       <c r="S30" s="4" t="s">
         <v>54</v>
       </c>
       <c r="T30" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="U30" s="4" t="s">
-        <v>54</v>
-      </c>
+      <c r="U30" s="4"/>
       <c r="V30" s="4" t="s">
         <v>54</v>
       </c>
       <c r="W30" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="X30" s="4" t="s">
-        <v>54</v>
-      </c>
+      <c r="X30" s="4"/>
       <c r="Y30" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="31" spans="2:25">
+      <c r="Z30" s="4"/>
+      <c r="AA30" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB30" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC30" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD30" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE30" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="2:31">
       <c r="B31" s="4" t="s">
         <v>76</v>
       </c>
@@ -4445,8 +5118,14 @@
       <c r="W31" s="4"/>
       <c r="X31" s="4"/>
       <c r="Y31" s="4"/>
-    </row>
-    <row r="32" spans="2:25">
+      <c r="Z31" s="4"/>
+      <c r="AA31" s="4"/>
+      <c r="AB31" s="4"/>
+      <c r="AC31" s="4"/>
+      <c r="AD31" s="4"/>
+      <c r="AE31" s="4"/>
+    </row>
+    <row r="32" spans="2:31">
       <c r="B32" s="4" t="s">
         <v>76</v>
       </c>
@@ -4519,8 +5198,26 @@
       <c r="Y32" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="33" spans="2:25">
+      <c r="Z32" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA32" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB32" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC32" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD32" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE32" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="2:31">
       <c r="B33" s="4" t="s">
         <v>76</v>
       </c>
@@ -4591,8 +5288,26 @@
       <c r="Y33" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="34" spans="2:25">
+      <c r="Z33" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA33" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB33" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC33" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD33" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE33" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="2:31">
       <c r="B34" s="4" t="s">
         <v>76</v>
       </c>
@@ -4627,8 +5342,14 @@
       <c r="W34" s="4"/>
       <c r="X34" s="4"/>
       <c r="Y34" s="4"/>
-    </row>
-    <row r="35" spans="2:25">
+      <c r="Z34" s="4"/>
+      <c r="AA34" s="4"/>
+      <c r="AB34" s="4"/>
+      <c r="AC34" s="4"/>
+      <c r="AD34" s="4"/>
+      <c r="AE34" s="4"/>
+    </row>
+    <row r="35" spans="2:31">
       <c r="B35" s="4" t="s">
         <v>76</v>
       </c>
@@ -4663,8 +5384,14 @@
       <c r="W35" s="4"/>
       <c r="X35" s="4"/>
       <c r="Y35" s="4"/>
-    </row>
-    <row r="36" spans="2:25">
+      <c r="Z35" s="4"/>
+      <c r="AA35" s="4"/>
+      <c r="AB35" s="4"/>
+      <c r="AC35" s="4"/>
+      <c r="AD35" s="4"/>
+      <c r="AE35" s="4"/>
+    </row>
+    <row r="36" spans="2:31">
       <c r="B36" s="4" t="s">
         <v>76</v>
       </c>
@@ -4699,8 +5426,14 @@
       <c r="W36" s="4"/>
       <c r="X36" s="4"/>
       <c r="Y36" s="4"/>
-    </row>
-    <row r="37" spans="2:25">
+      <c r="Z36" s="4"/>
+      <c r="AA36" s="4"/>
+      <c r="AB36" s="4"/>
+      <c r="AC36" s="4"/>
+      <c r="AD36" s="4"/>
+      <c r="AE36" s="4"/>
+    </row>
+    <row r="37" spans="2:31">
       <c r="B37" s="4" t="s">
         <v>76</v>
       </c>
@@ -4735,8 +5468,14 @@
       <c r="W37" s="4"/>
       <c r="X37" s="4"/>
       <c r="Y37" s="4"/>
-    </row>
-    <row r="38" spans="2:25">
+      <c r="Z37" s="4"/>
+      <c r="AA37" s="4"/>
+      <c r="AB37" s="4"/>
+      <c r="AC37" s="4"/>
+      <c r="AD37" s="4"/>
+      <c r="AE37" s="4"/>
+    </row>
+    <row r="38" spans="2:31">
       <c r="B38" s="4" t="s">
         <v>76</v>
       </c>
@@ -4771,8 +5510,14 @@
       <c r="W38" s="4"/>
       <c r="X38" s="4"/>
       <c r="Y38" s="4"/>
-    </row>
-    <row r="39" spans="2:25">
+      <c r="Z38" s="4"/>
+      <c r="AA38" s="4"/>
+      <c r="AB38" s="4"/>
+      <c r="AC38" s="4"/>
+      <c r="AD38" s="4"/>
+      <c r="AE38" s="4"/>
+    </row>
+    <row r="39" spans="2:31">
       <c r="B39" s="4" t="s">
         <v>76</v>
       </c>
@@ -4823,8 +5568,22 @@
       <c r="W39" s="4"/>
       <c r="X39" s="4"/>
       <c r="Y39" s="4"/>
-    </row>
-    <row r="40" spans="2:25">
+      <c r="Z39" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA39" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB39" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC39" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD39" s="4"/>
+      <c r="AE39" s="4"/>
+    </row>
+    <row r="40" spans="2:31">
       <c r="B40" s="4" t="s">
         <v>76</v>
       </c>
@@ -4859,8 +5618,14 @@
       <c r="W40" s="4"/>
       <c r="X40" s="4"/>
       <c r="Y40" s="4"/>
-    </row>
-    <row r="41" spans="2:25">
+      <c r="Z40" s="4"/>
+      <c r="AA40" s="4"/>
+      <c r="AB40" s="4"/>
+      <c r="AC40" s="4"/>
+      <c r="AD40" s="4"/>
+      <c r="AE40" s="4"/>
+    </row>
+    <row r="41" spans="2:31">
       <c r="B41" s="4" t="s">
         <v>76</v>
       </c>
@@ -4895,8 +5660,14 @@
       <c r="W41" s="4"/>
       <c r="X41" s="4"/>
       <c r="Y41" s="4"/>
-    </row>
-    <row r="42" spans="2:25">
+      <c r="Z41" s="4"/>
+      <c r="AA41" s="4"/>
+      <c r="AB41" s="4"/>
+      <c r="AC41" s="4"/>
+      <c r="AD41" s="4"/>
+      <c r="AE41" s="4"/>
+    </row>
+    <row r="42" spans="2:31">
       <c r="B42" s="4" t="s">
         <v>76</v>
       </c>
@@ -4931,8 +5702,14 @@
       <c r="W42" s="4"/>
       <c r="X42" s="4"/>
       <c r="Y42" s="4"/>
-    </row>
-    <row r="43" spans="2:25">
+      <c r="Z42" s="4"/>
+      <c r="AA42" s="4"/>
+      <c r="AB42" s="4"/>
+      <c r="AC42" s="4"/>
+      <c r="AD42" s="4"/>
+      <c r="AE42" s="4"/>
+    </row>
+    <row r="43" spans="2:31">
       <c r="B43" s="4" t="s">
         <v>76</v>
       </c>
@@ -4967,8 +5744,16 @@
       <c r="W43" s="4"/>
       <c r="X43" s="4"/>
       <c r="Y43" s="4"/>
-    </row>
-    <row r="44" spans="2:25">
+      <c r="Z43" s="4"/>
+      <c r="AA43" s="4"/>
+      <c r="AB43" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC43" s="4"/>
+      <c r="AD43" s="4"/>
+      <c r="AE43" s="4"/>
+    </row>
+    <row r="44" spans="2:31">
       <c r="B44" s="4" t="s">
         <v>76</v>
       </c>
@@ -5003,8 +5788,16 @@
       <c r="W44" s="4"/>
       <c r="X44" s="4"/>
       <c r="Y44" s="4"/>
-    </row>
-    <row r="45" spans="2:25">
+      <c r="Z44" s="4"/>
+      <c r="AA44" s="4"/>
+      <c r="AB44" s="4"/>
+      <c r="AC44" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD44" s="4"/>
+      <c r="AE44" s="4"/>
+    </row>
+    <row r="45" spans="2:31">
       <c r="B45" s="4" t="s">
         <v>76</v>
       </c>
@@ -5039,8 +5832,16 @@
       <c r="W45" s="4"/>
       <c r="X45" s="4"/>
       <c r="Y45" s="4"/>
-    </row>
-    <row r="46" spans="2:25">
+      <c r="Z45" s="4"/>
+      <c r="AA45" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB45" s="4"/>
+      <c r="AC45" s="4"/>
+      <c r="AD45" s="4"/>
+      <c r="AE45" s="4"/>
+    </row>
+    <row r="46" spans="2:31">
       <c r="B46" s="4" t="s">
         <v>76</v>
       </c>
@@ -5075,8 +5876,14 @@
       <c r="Y46" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="47" spans="2:25">
+      <c r="Z46" s="4"/>
+      <c r="AA46" s="4"/>
+      <c r="AB46" s="4"/>
+      <c r="AC46" s="4"/>
+      <c r="AD46" s="4"/>
+      <c r="AE46" s="4"/>
+    </row>
+    <row r="47" spans="2:31">
       <c r="B47" s="4" t="s">
         <v>76</v>
       </c>
@@ -5111,8 +5918,14 @@
       <c r="W47" s="4"/>
       <c r="X47" s="4"/>
       <c r="Y47" s="4"/>
-    </row>
-    <row r="48" spans="2:25">
+      <c r="Z47" s="4"/>
+      <c r="AA47" s="4"/>
+      <c r="AB47" s="4"/>
+      <c r="AC47" s="4"/>
+      <c r="AD47" s="4"/>
+      <c r="AE47" s="4"/>
+    </row>
+    <row r="48" spans="2:31">
       <c r="B48" s="4" t="s">
         <v>76</v>
       </c>
@@ -5147,8 +5960,14 @@
       <c r="W48" s="4"/>
       <c r="X48" s="4"/>
       <c r="Y48" s="4"/>
-    </row>
-    <row r="49" spans="2:25">
+      <c r="Z48" s="4"/>
+      <c r="AA48" s="4"/>
+      <c r="AB48" s="4"/>
+      <c r="AC48" s="4"/>
+      <c r="AD48" s="4"/>
+      <c r="AE48" s="4"/>
+    </row>
+    <row r="49" spans="2:31">
       <c r="B49" s="4" t="s">
         <v>76</v>
       </c>
@@ -5183,8 +6002,14 @@
       <c r="W49" s="4"/>
       <c r="X49" s="4"/>
       <c r="Y49" s="4"/>
-    </row>
-    <row r="50" spans="2:25">
+      <c r="Z49" s="4"/>
+      <c r="AA49" s="4"/>
+      <c r="AB49" s="4"/>
+      <c r="AC49" s="4"/>
+      <c r="AD49" s="4"/>
+      <c r="AE49" s="4"/>
+    </row>
+    <row r="50" spans="2:31">
       <c r="B50" s="4" t="s">
         <v>76</v>
       </c>
@@ -5219,8 +6044,14 @@
       </c>
       <c r="X50" s="4"/>
       <c r="Y50" s="4"/>
-    </row>
-    <row r="51" spans="2:25">
+      <c r="Z50" s="4"/>
+      <c r="AA50" s="4"/>
+      <c r="AB50" s="4"/>
+      <c r="AC50" s="4"/>
+      <c r="AD50" s="4"/>
+      <c r="AE50" s="4"/>
+    </row>
+    <row r="51" spans="2:31">
       <c r="B51" s="4" t="s">
         <v>76</v>
       </c>
@@ -5255,8 +6086,14 @@
       <c r="Y51" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="52" spans="2:25">
+      <c r="Z51" s="4"/>
+      <c r="AA51" s="4"/>
+      <c r="AB51" s="4"/>
+      <c r="AC51" s="4"/>
+      <c r="AD51" s="4"/>
+      <c r="AE51" s="4"/>
+    </row>
+    <row r="52" spans="2:31">
       <c r="B52" s="4" t="s">
         <v>76</v>
       </c>
@@ -5293,8 +6130,14 @@
       <c r="W52" s="4"/>
       <c r="X52" s="4"/>
       <c r="Y52" s="4"/>
-    </row>
-    <row r="53" spans="2:25">
+      <c r="Z52" s="4"/>
+      <c r="AA52" s="4"/>
+      <c r="AB52" s="4"/>
+      <c r="AC52" s="4"/>
+      <c r="AD52" s="4"/>
+      <c r="AE52" s="4"/>
+    </row>
+    <row r="53" spans="2:31">
       <c r="B53" s="4" t="s">
         <v>76</v>
       </c>
@@ -5327,8 +6170,16 @@
       <c r="W53" s="4"/>
       <c r="X53" s="4"/>
       <c r="Y53" s="4"/>
-    </row>
-    <row r="54" spans="2:25">
+      <c r="Z53" s="4"/>
+      <c r="AA53" s="4"/>
+      <c r="AB53" s="4"/>
+      <c r="AC53" s="4"/>
+      <c r="AD53" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE53" s="4"/>
+    </row>
+    <row r="54" spans="2:31">
       <c r="B54" s="4" t="s">
         <v>76</v>
       </c>
@@ -5367,8 +6218,16 @@
       <c r="Y54" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="55" spans="2:25">
+      <c r="Z54" s="4"/>
+      <c r="AA54" s="4"/>
+      <c r="AB54" s="4"/>
+      <c r="AC54" s="4"/>
+      <c r="AD54" s="4"/>
+      <c r="AE54" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55" spans="2:31">
       <c r="B55" s="4" t="s">
         <v>76</v>
       </c>
@@ -5415,6 +6274,18 @@
       <c r="Y55" s="4" t="s">
         <v>54</v>
       </c>
+      <c r="Z55" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA55" s="4"/>
+      <c r="AB55" s="4"/>
+      <c r="AC55" s="4"/>
+      <c r="AD55" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE55" s="4" t="s">
+        <v>54</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>